<commit_message>
PN1: Data Simulation and Initial Reactable demo
</commit_message>
<xml_diff>
--- a/Prototypes/PN_1/data/Lit Review Matrix - Upstream Policies and Health Outcomes 6-28-21.xlsx
+++ b/Prototypes/PN_1/data/Lit Review Matrix - Upstream Policies and Health Outcomes 6-28-21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranli\Desktop\Git local\BCHC Policy Review\Prototypes\PN_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranli\Desktop\Git local\BCHC Policy Review\Prototypes\PN_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0260458D-4086-4900-979C-69C8309EF30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857A0563-7555-4A99-8009-9CA51E392676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{91655CBE-7744-41B9-AECB-CA897763B8F2}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{91655CBE-7744-41B9-AECB-CA897763B8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="matrix" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="68">
   <si>
     <t>Chronic diseases</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Policy Group</t>
   </si>
   <si>
-    <t>Outcome Group</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
@@ -157,6 +154,93 @@
   </si>
   <si>
     <t>P-value</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income </t>
+  </si>
+  <si>
+    <t>Discrimination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Housing </t>
+  </si>
+  <si>
+    <t>Community Investment</t>
+  </si>
+  <si>
+    <t>Public schooling Investments</t>
+  </si>
+  <si>
+    <t>Paid Leave</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Increased Childcare</t>
+  </si>
+  <si>
+    <t>Education and Childcare</t>
+  </si>
+  <si>
+    <t>Inclusive labor policies</t>
+  </si>
+  <si>
+    <t>Benefitial Housing Policy</t>
+  </si>
+  <si>
+    <t>Equity based policies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increased Isurance access </t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Racial discrimination</t>
+  </si>
+  <si>
+    <t>Inclusive economic policy</t>
+  </si>
+  <si>
+    <t>Equity based Built Environment policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policy Short </t>
+  </si>
+  <si>
+    <t>Equity based Tax Policy</t>
+  </si>
+  <si>
+    <t>Conservative Tax Policy</t>
+  </si>
+  <si>
+    <t>Increased Voting Access</t>
+  </si>
+  <si>
+    <t>Decreased Voting Access</t>
+  </si>
+  <si>
+    <t>Life Expectancy</t>
+  </si>
+  <si>
+    <t>Prior Belief effect on health Outcomes</t>
+  </si>
+  <si>
+    <t>Outcome Short</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior Z Score </t>
   </si>
 </sst>
 </file>
@@ -256,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -326,6 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76B3283-73AF-4BC5-8FB9-52DC3BCE3176}">
   <dimension ref="B2:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -980,16 +1065,16 @@
         <v>32</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>38</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="120" x14ac:dyDescent="0.25">
@@ -1003,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="18"/>
@@ -1056,117 +1141,294 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FF43D0-345F-4973-BAC3-C250ABD5562A}">
-  <dimension ref="B2:C17"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B5:B8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="44" style="10" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="10" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="10"/>
+    <col min="2" max="2" width="22.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" style="10" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="D2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="14"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="D3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="14"/>
-    </row>
-    <row r="5" spans="2:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="D4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="D5" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="D6" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="14"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="D7" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="D8" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="14"/>
-    </row>
-    <row r="10" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="14"/>
-    </row>
-    <row r="11" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="D9" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="14"/>
-    </row>
-    <row r="12" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
+      <c r="D10" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="14">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="2:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
+      <c r="D11" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="14"/>
-    </row>
-    <row r="14" spans="2:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
+      <c r="D12" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="14"/>
-    </row>
-    <row r="15" spans="2:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="D13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="14"/>
-    </row>
-    <row r="16" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="D14" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="14">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="14"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="14"/>
+      <c r="D16" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="14">
+        <v>-0.9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1179,81 +1441,102 @@
   <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>34</v>
+      <c r="C2" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="15" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="15" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="18"/>
-    </row>
-    <row r="6" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C5" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="18"/>
-    </row>
-    <row r="8" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18"/>
-    </row>
-    <row r="9" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C8" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-    </row>
-    <row r="11" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C10" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="15" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="15" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1261,21 +1544,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B33ACE731AB07341AE5126C3DA9F4C14" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="26e6ff49344acef95e2064f655fa0c8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="add7b089-4dde-484e-a58b-af385cd258ee" xmlns:ns3="2668201c-984e-41c3-be1f-d1fe4f7774bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="131adc71cac139061e16379c73acc269" ns2:_="" ns3:_="">
     <xsd:import namespace="add7b089-4dde-484e-a58b-af385cd258ee"/>
@@ -1498,15 +1772,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FB8F18E-5FC7-49C0-8742-4EBD888DA06A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354C80EB-C06E-464C-AD3C-7B13542B0A24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1515,7 +1790,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D69B468-98E1-4AD8-B5C6-1FF56939E88B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1532,4 +1807,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FB8F18E-5FC7-49C0-8742-4EBD888DA06A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>